<commit_message>
Added the Alphafold 3 job submission
</commit_message>
<xml_diff>
--- a/Protein_Seq_List.xlsx
+++ b/Protein_Seq_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my_driv\Fortune\Education\University\Masters\NTU\Lab_Projects\Nege\Automation\ProteinFold_Pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94F426E-22BF-467C-B591-31BEFA1407C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB4FC06-2402-421B-96AD-278D3995686D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2565" windowWidth="29040" windowHeight="15720" xr2:uid="{3E744B27-A762-4403-90C4-99D11043315A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{3E744B27-A762-4403-90C4-99D11043315A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,25 +36,424 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Seq_Name</t>
-  </si>
-  <si>
-    <t>SNAI1_and_SNAI1_187R_sequences</t>
-  </si>
-  <si>
-    <t>QLSEAKDLQARKAFNCKYCNKEYLSLGALKMHIRSHTLPCVCGTCGKAFSRPWLLQGHVRTHTGEKPFSCPHC</t>
-  </si>
-  <si>
-    <t>Wild</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QLSEARDLQARKAFNCKYCNKEYLSLGALKMHIRSHTLPCVCGTCGKAFSRPWLLQGHVRTHTGEKPFSCPHC </t>
-  </si>
-  <si>
-    <r>
-      <t>QLSEAKDLQARKAFNCKYCNKEYLSLGALKMHIRSHTLPCVCGTCG</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>Protein_name</t>
+  </si>
+  <si>
+    <t>Protein_sequence</t>
+  </si>
+  <si>
+    <t>Protein_region_of_interest_(ROI)</t>
+  </si>
+  <si>
+    <t>DNA_region_of_interest_(ROI)</t>
+  </si>
+  <si>
+    <t>SNAI1-187R-154_230</t>
+  </si>
+  <si>
+    <r>
+      <t>FNCKYCNKEYLSLGALKMHI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SHTLPCVCGTCG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFSRP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>WL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LQG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>VRTHTGE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PFSCPHCS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFADR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">H </t>
+    </r>
+  </si>
+  <si>
+    <t>R174-R187-W193-L194-H198-K206-R215-S221-N222-R224-H226-T229</t>
+  </si>
+  <si>
+    <t>CACCTG</t>
+  </si>
+  <si>
+    <t>SNAI1-187K-154_230</t>
+  </si>
+  <si>
+    <r>
+      <t>FNCKYCNKEYLSLGALKMHI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SHTLPCVCGTCG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFSRP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>WL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LQG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>VRTHTGE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PFSCPHCS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFADR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R174-</t>
     </r>
     <r>
       <rPr>
@@ -63,56 +462,208 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>R187-W193-L194-H198-K206-R215-S221-N222-R224-H226-T229</t>
+    </r>
+  </si>
+  <si>
+    <t>SNAI1-187D-154_230</t>
+  </si>
+  <si>
+    <r>
+      <t>FNCKYCNKEYLSLGALKMHI</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>R</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>AFSRPWLLQGHVRTHTGEKPFSCPHC</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>QLSEARDLQARKAFNCKYCNKEYLSLGALKMHIRSHTLPCVCGTCG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>SHTLPCVCGTCG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFSRP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>WL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LQG</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>VRTHTGE</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PFSCPHCS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>R</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>AFSRPWLLQGHVRTHTGEKPFSCPHC</t>
-    </r>
-  </si>
-  <si>
-    <t>R146</t>
-  </si>
-  <si>
-    <t>R187</t>
-  </si>
-  <si>
-    <t>2R</t>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AFADR</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>AHLQ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">H </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R174-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>W193-L194-H198-K206-R215-S221-N222-R224-T229</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,11 +685,30 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,7 +719,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,15 +727,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,59 +1104,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504D0461-63F0-4B26-AFA6-454E106E5722}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="92.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
+    <row r="3" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+    <row r="4" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>